<commit_message>
Report able to generat and new ordering featur implementd
</commit_message>
<xml_diff>
--- a/Resource_TestData/TestData.xlsx
+++ b/Resource_TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="12885" windowHeight="5700"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15570" windowHeight="4830"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -548,6 +548,9 @@
       </c>
       <c r="J2" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12">

</xml_diff>

<commit_message>
ordering script is done
</commit_message>
<xml_diff>
--- a/Resource_TestData/TestData.xlsx
+++ b/Resource_TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16650" windowHeight="3615"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16650" windowHeight="5850"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -459,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -545,6 +545,9 @@
       </c>
       <c r="J2" t="s">
         <v>27</v>
+      </c>
+      <c r="K2">
+        <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:12">

</xml_diff>

<commit_message>
script changes of order placeing
</commit_message>
<xml_diff>
--- a/Resource_TestData/TestData.xlsx
+++ b/Resource_TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16650" windowHeight="5850"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17790" windowHeight="5025"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>maggi</t>
+  </si>
+  <si>
+    <t>login_as_counter_and_place_an_order</t>
   </si>
 </sst>
 </file>
@@ -459,14 +462,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
@@ -616,11 +619,21 @@
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>

</xml_diff>